<commit_message>
Working download and chatting functionality
</commit_message>
<xml_diff>
--- a/backend/myproject/abc.xlsx
+++ b/backend/myproject/abc.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Professions" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Football" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Football Goals" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cricket Runs" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,133 +437,258 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Profession</t>
+          <t>Rank</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Average Salary Range</t>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Season</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Goals</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Physician</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$171,285 to $282,496</t>
-        </is>
+          <t>Lionel Messi</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2011/12</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Solar Sales Representative</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$90,510 to $121,504</t>
-        </is>
+          <t>Ferenc Deak</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Szentlorinci</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1945/46</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>66</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Medical Director</t>
-        </is>
+      <c r="A4" t="n">
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>$302,490 to $363,214</t>
-        </is>
+          <t>Gerd Muller</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Bayern Munich</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1972/73</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>66</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Dentist</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$175,292 to $220,861</t>
-        </is>
+          <t>Dixie Dean</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Everton</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1927/28</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Psychiatrist</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>$242,206 to $296,048</t>
-        </is>
+          <t>Cristiano Ronaldo</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2014/15</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>61</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Principal Software Engineer</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$119,335 to $142,721</t>
-        </is>
+          <t>Cristiano Ronaldo</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2011/12</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Outside Sales Representative</t>
-        </is>
+      <c r="A8" t="n">
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>$90,833 to $122,099</t>
-        </is>
+          <t>Lionel Messi</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2012/13</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Chief Financial Officer (CFO)</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>$338,470 to $579,175</t>
-        </is>
+          <t>Ferenc Deak</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ferencvaros</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1948/49</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Veterinarian Radiologist</t>
-        </is>
+      <c r="A10" t="n">
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>$160,000 to $287,000</t>
-        </is>
+          <t>Luis Suarez</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2015/16</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Endodontist</t>
-        </is>
+      <c r="A11" t="n">
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>$177,156 to $223,078</t>
-        </is>
+          <t>Lionel Messi</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2014/15</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -577,7 +702,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -588,33 +713,133 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Player</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Goals</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Season</t>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Runs</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Lionel Messi</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>73</v>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>KC Sangakkara</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2011-12</t>
-        </is>
+          <t>SL</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>2868</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>RT Ponting</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>AUS/ICC</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2833</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>V Kohli</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>IND</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2818</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>V Kohli</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>IND</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2735</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>KS Williamson</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NZ</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>2692</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Downlaod Functionality Added Successfully
</commit_message>
<xml_diff>
--- a/backend/myproject/abc.xlsx
+++ b/backend/myproject/abc.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rivers" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ballon dOr" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Football" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cricket" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,66 +437,277 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Country</t>
+          <t>Rank</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Major Rivers</t>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Season</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Goals</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Russia</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>36</v>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Lionel Messi</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2011/12</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>73 Goals</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Brazil</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>24</v>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Ferenc Deak</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Szentlorinci</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1945/46</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>66 Goals</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>12</v>
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Gerd Muller</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Bayern Munich</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1972/73</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>66 Goals</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>China</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Extensive</t>
+          <t>Dixie Dean</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Everton</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1927/28</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>63 Goals</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Extensive</t>
+          <t>Cristiano Ronaldo</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2014/15</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>61 Goals</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Cristiano Ronaldo</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2011/12</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>60 Goals</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Lionel Messi</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2012/13</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>60 Goals</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Ferenc Deak</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ferencvaros</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1948/49</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>59 Goals</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Luis Suarez</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2015/16</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>59 Goals</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Lionel Messi</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2014/15</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>58 Goals</t>
         </is>
       </c>
     </row>
@@ -511,7 +722,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,93 +733,133 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Player</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Awards</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Years</t>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Runs</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Lionel Messi</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>8</v>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>KC Sangakkara</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2009, 2010, 2011, 2012, 2015, 2019, 2021, 2023</t>
-        </is>
+          <t>SL</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>2868</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2013</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Cristiano Ronaldo</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>RT Ponting</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>AUS/ICC</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2833</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>V Kohli</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>IND</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2818</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>V Kohli</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>IND</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2735</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2008, 2013, 2014, 2016, 2017</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Michel Platini</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>1983, 1984, 1985</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Johann Cruyff</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1971, 1973, 1974</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Marco van Basten</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>3</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>KS Williamson</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1988, 1989, 1992</t>
-        </is>
+          <t>NZ</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>2692</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Env File is Added
</commit_message>
<xml_diff>
--- a/backend/myproject/abc.xlsx
+++ b/backend/myproject/abc.xlsx
@@ -7,8 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Football" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cricket" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Major Rivers" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ballon d'Or Awards" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Shoes Under $10" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,277 +438,66 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Rank</t>
+          <t>Country</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Player</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Team</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Season</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Goals</t>
+          <t>Major Rivers</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Lionel Messi</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Barcelona</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2011/12</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>73 Goals</t>
-        </is>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Russia</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Ferenc Deak</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Szentlorinci</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1945/46</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>66 Goals</t>
-        </is>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Brazil</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Gerd Muller</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Bayern Munich</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1972/73</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>66 Goals</t>
-        </is>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Dixie Dean</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Everton</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>1927/28</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>63 Goals</t>
+          <t>Extensive network</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cristiano Ronaldo</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Real Madrid</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2014/15</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>61 Goals</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Cristiano Ronaldo</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Real Madrid</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2011/12</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>60 Goals</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Lionel Messi</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Barcelona</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2012/13</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>60 Goals</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Ferenc Deak</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Ferencvaros</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>1948/49</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>59 Goals</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Luis Suarez</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Barcelona</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2015/16</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>59 Goals</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Lionel Messi</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Barcelona</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2014/15</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>58 Goals</t>
+          <t>Extensive network</t>
         </is>
       </c>
     </row>
@@ -722,7 +512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -733,133 +523,219 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Rank</t>
+          <t>Player</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Player</t>
+          <t>Awards</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Country</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Runs</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Year</t>
+          <t>Years</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>KC Sangakkara</t>
-        </is>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Lionel Messi</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>8</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SL</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>2868</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2013</v>
+          <t>2009, 2010, 2011, 2012, 2015, 2019, 2021, 2023</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>RT Ponting</t>
-        </is>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cristiano Ronaldo</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>AUS/ICC</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>2833</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2005</v>
+          <t>2008, 2013, 2014, 2016, 2017</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Michel Platini</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>V Kohli</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IND</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>2818</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2017</v>
+          <t>1983, 1984, 1985</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>V Kohli</t>
-        </is>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Johan Cruyff</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>IND</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>2735</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2018</v>
+          <t>1971, 1973, 1974</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>KS Williamson</t>
-        </is>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Marco van Basten</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NZ</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>2692</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2015</v>
+          <t>1988, 1989, 1992</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Image URL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Vsufim Quick-Dry Water Sports Barefoot Shoes Aqua Socks for Swim Beach Pool Surf Yoga for Women Men</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>5.94</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51FCX+Z8X8L._AC_UL320_.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Limberun Water Shoes for Women Men Swim Beach Shoes</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>9.98</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/617fZ5q3arL._AC_UL320_.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ATHMILE Quick-Dry Aqua Socks Swim Beach Barefoot Yoga Exercise Wear Sport Accessories Pool Camping Must Haves Adult Youth Size</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>6.99</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61GzQfBa+lL._AC_UL320_.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Laura Ashley Soft Terry Knot Scuff Slippers for Women</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>6.99</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71PzOIxOwcL._AC_UL320_.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cosyone1997 Cute Animal Slippers for Kids Girls Women</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71qqzJ5O4IL._AC_UL320_.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>WateLves Womens and Mens Kids Water Shoes Barefoot Quick-Dry Aqua Socks for Beach Swim Surf Yoga Exercise</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>7.96</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51LONA7bXKL._AC_UL320_.jpg</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>